<commit_message>
uploading code with renamed folders
</commit_message>
<xml_diff>
--- a/properties/excel_database.xlsx
+++ b/properties/excel_database.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80470bce47444d73/Documents/GitHub/json_to_excel/properties/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_832E2B7E52D7FEBE891C875A0AEF671161B4F935" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87F19497-AB6F-4A1B-9F37-FEB37D1FF29A}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Index</t>
   </si>
@@ -24,72 +30,12 @@
   <si>
     <t>Status</t>
   </si>
-  <si>
-    <t>ABC_1</t>
-  </si>
-  <si>
-    <t>ABC_2</t>
-  </si>
-  <si>
-    <t>ABC_3</t>
-  </si>
-  <si>
-    <t>ABC_4</t>
-  </si>
-  <si>
-    <t>ABC_5</t>
-  </si>
-  <si>
-    <t>ABC_6</t>
-  </si>
-  <si>
-    <t>ABC_7</t>
-  </si>
-  <si>
-    <t>ABC_8</t>
-  </si>
-  <si>
-    <t>ABC_9</t>
-  </si>
-  <si>
-    <t>ABC_10</t>
-  </si>
-  <si>
-    <t>sample_status_1</t>
-  </si>
-  <si>
-    <t>sample_status_2</t>
-  </si>
-  <si>
-    <t>sample_status_3</t>
-  </si>
-  <si>
-    <t>sample_status_4</t>
-  </si>
-  <si>
-    <t>sample_status_5</t>
-  </si>
-  <si>
-    <t>sample_status_6</t>
-  </si>
-  <si>
-    <t>sample_status_7</t>
-  </si>
-  <si>
-    <t>sample_status_8</t>
-  </si>
-  <si>
-    <t>sample_status_9</t>
-  </si>
-  <si>
-    <t>sample_status_10</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,6 +98,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -198,7 +152,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,9 +184,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,6 +236,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,14 +429,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -457,226 +447,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding logging and exception handling
</commit_message>
<xml_diff>
--- a/properties/excel_database.xlsx
+++ b/properties/excel_database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/80470bce47444d73/Documents/GitHub/json_to_excel/properties/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\OneDrive\Documents\GitHub\json_to_excel\properties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_832E2B7E52D7FEBE891C875A0AEF671161B4F935" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87F19497-AB6F-4A1B-9F37-FEB37D1FF29A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8872202F-4EB9-4C41-8EC1-E0EA3448838E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>